<commit_message>
Utvikling og rydding - Tilpassa førebuing av studiebarometerdata til 2024-data - lagt til bibliotek for å lage interaktive plott - oppdatert filer for programnamn o.l.
</commit_message>
<xml_diff>
--- a/base/OsloMet_paraplyprogram.xlsx
+++ b/base/OsloMet_paraplyprogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCC23C44-DBA2-475C-AEE9-C2B212F17956}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E2B19F-BDA5-4ECC-AED0-B9B4923922E1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>Studieprogramkode</t>
   </si>
@@ -213,7 +213,13 @@
     <t>MSFD</t>
   </si>
   <si>
-    <t>MASPSYK</t>
+    <t>MASY</t>
+  </si>
+  <si>
+    <t>MASKA</t>
+  </si>
+  <si>
+    <t>Masterstudium i spesialsykepleie til akutt og kritisk syke pasienter med spesialisering i kardiologisk sykepleie (D)</t>
   </si>
 </sst>
 </file>
@@ -531,16 +537,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -925,13 +931,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -940,7 +946,7 @@
         <v>120</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,10 +954,10 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -968,10 +974,10 @@
         <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -988,10 +994,10 @@
         <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -1005,13 +1011,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -1020,7 +1026,7 @@
         <v>120</v>
       </c>
       <c r="F24">
-        <v>0.67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1028,10 +1034,10 @@
         <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
@@ -1048,10 +1054,10 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -1068,10 +1074,10 @@
         <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -1083,10 +1089,31 @@
         <v>0.67</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>120</v>
+      </c>
+      <c r="F28">
+        <v>0.67</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B21:F27">
-    <sortCondition descending="1" ref="F20:F27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B22:F28">
+    <sortCondition descending="1" ref="F21:F28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Utvikling – La til funksjon for å kunne slå saman paraplyprogram – Korrigert indeksar der grunnlaget er endra – Koding av nye variablar i Studiebarometeret – La til kontroll for manglande variabel i datasett til samanlikning – La til filter for å handtere tidsvariabel ved samanslåtte program – La til kode for å levere data til Styringsportalen
</commit_message>
<xml_diff>
--- a/base/OsloMet_paraplyprogram.xlsx
+++ b/base/OsloMet_paraplyprogram.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E2B19F-BDA5-4ECC-AED0-B9B4923922E1}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B791EC-F160-4A32-94A9-C93887858CF3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
   <si>
     <t>Studieprogramkode</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>Masterstudium i spesialsykepleie til akutt og kritisk syke pasienter med spesialisering i kardiologisk sykepleie (D)</t>
+  </si>
+  <si>
+    <t>Paraplynamn</t>
+  </si>
+  <si>
+    <t>MAVIT Helsevitenskap</t>
+  </si>
+  <si>
+    <t>MASY Spesialsykepleie</t>
+  </si>
+  <si>
+    <t>MSFH Sosialfag (H)</t>
+  </si>
+  <si>
+    <t>MSFD Sosialfag (D)</t>
   </si>
 </sst>
 </file>
@@ -272,6 +287,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9345AFD5-DC4B-4E57-96B1-4032661EA08A}" name="Table1" displayName="Table1" ref="A1:G28" totalsRowShown="0">
+  <autoFilter ref="A1:G28" xr:uid="{9345AFD5-DC4B-4E57-96B1-4032661EA08A}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{3E888C8F-04E8-4758-9FD8-E2C7C7B88714}" name="Paraplyvennleg_kode"/>
+    <tableColumn id="2" xr3:uid="{C6E1CC84-C33F-4241-AE2A-40A8CE17C98D}" name="Studieprogramkode"/>
+    <tableColumn id="7" xr3:uid="{3C4504EF-B2A1-4576-9CD7-42FCE9B0EF2C}" name="Paraplynamn"/>
+    <tableColumn id="3" xr3:uid="{E0C149E3-B58C-459B-ACB6-4650289AED7A}" name="Studietilbod"/>
+    <tableColumn id="4" xr3:uid="{86E3E6BA-E244-45F5-BAD8-A77C56F40E2D}" name="Nivåkode"/>
+    <tableColumn id="5" xr3:uid="{B2EE1995-942F-444B-AE97-757B28874219}" name="Studiepoeng"/>
+    <tableColumn id="6" xr3:uid="{9A18D7BA-2469-4D7B-9AA7-85C83C984999}" name="Andel av heltid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,19 +568,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="104" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -557,19 +592,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -577,19 +615,22 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2">
-        <v>120</v>
+      <c r="E2" t="s">
+        <v>32</v>
       </c>
       <c r="F2">
+        <v>120</v>
+      </c>
+      <c r="G2">
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -597,19 +638,22 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>120</v>
+      <c r="E3" t="s">
+        <v>32</v>
       </c>
       <c r="F3">
+        <v>120</v>
+      </c>
+      <c r="G3">
         <v>0.67</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -617,19 +661,22 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4">
-        <v>120</v>
+      <c r="E4" t="s">
+        <v>32</v>
       </c>
       <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -637,19 +684,22 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5">
-        <v>120</v>
+      <c r="E5" t="s">
+        <v>32</v>
       </c>
       <c r="F5">
+        <v>120</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -657,19 +707,22 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>120</v>
+      <c r="E6" t="s">
+        <v>32</v>
       </c>
       <c r="F6">
+        <v>120</v>
+      </c>
+      <c r="G6">
         <v>0.67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -677,19 +730,22 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7">
-        <v>120</v>
+      <c r="E7" t="s">
+        <v>32</v>
       </c>
       <c r="F7">
+        <v>120</v>
+      </c>
+      <c r="G7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -697,19 +753,22 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8">
-        <v>120</v>
+      <c r="E8" t="s">
+        <v>32</v>
       </c>
       <c r="F8">
+        <v>120</v>
+      </c>
+      <c r="G8">
         <v>0.67</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -717,19 +776,22 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9">
-        <v>120</v>
+      <c r="E9" t="s">
+        <v>32</v>
       </c>
       <c r="F9">
+        <v>120</v>
+      </c>
+      <c r="G9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -737,19 +799,22 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10">
-        <v>120</v>
+      <c r="E10" t="s">
+        <v>32</v>
       </c>
       <c r="F10">
+        <v>120</v>
+      </c>
+      <c r="G10">
         <v>0.67</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -757,19 +822,22 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11">
-        <v>120</v>
+      <c r="E11" t="s">
+        <v>32</v>
       </c>
       <c r="F11">
+        <v>120</v>
+      </c>
+      <c r="G11">
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -777,19 +845,22 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12">
-        <v>120</v>
+      <c r="E12" t="s">
+        <v>32</v>
       </c>
       <c r="F12">
+        <v>120</v>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -797,19 +868,22 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13">
-        <v>120</v>
+      <c r="E13" t="s">
+        <v>32</v>
       </c>
       <c r="F13">
+        <v>120</v>
+      </c>
+      <c r="G13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -817,19 +891,22 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14">
-        <v>120</v>
+      <c r="E14" t="s">
+        <v>32</v>
       </c>
       <c r="F14">
+        <v>120</v>
+      </c>
+      <c r="G14">
         <v>0.67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -837,19 +914,22 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15">
-        <v>120</v>
+      <c r="E15" t="s">
+        <v>32</v>
       </c>
       <c r="F15">
+        <v>120</v>
+      </c>
+      <c r="G15">
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -857,19 +937,22 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16">
-        <v>120</v>
+      <c r="E16" t="s">
+        <v>32</v>
       </c>
       <c r="F16">
+        <v>120</v>
+      </c>
+      <c r="G16">
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -877,19 +960,22 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17">
-        <v>120</v>
+      <c r="E17" t="s">
+        <v>32</v>
       </c>
       <c r="F17">
+        <v>120</v>
+      </c>
+      <c r="G17">
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -897,19 +983,22 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
         <v>40</v>
       </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18">
-        <v>120</v>
+      <c r="E18" t="s">
+        <v>32</v>
       </c>
       <c r="F18">
+        <v>120</v>
+      </c>
+      <c r="G18">
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -917,19 +1006,22 @@
         <v>41</v>
       </c>
       <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19">
-        <v>120</v>
+      <c r="E19" t="s">
+        <v>32</v>
       </c>
       <c r="F19">
+        <v>120</v>
+      </c>
+      <c r="G19">
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -937,19 +1029,22 @@
         <v>63</v>
       </c>
       <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20">
-        <v>120</v>
+      <c r="E20" t="s">
+        <v>32</v>
       </c>
       <c r="F20">
+        <v>120</v>
+      </c>
+      <c r="G20">
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -957,19 +1052,22 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21">
-        <v>120</v>
+      <c r="E21" t="s">
+        <v>32</v>
       </c>
       <c r="F21">
+        <v>120</v>
+      </c>
+      <c r="G21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -977,19 +1075,22 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
         <v>49</v>
       </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22">
-        <v>120</v>
+      <c r="E22" t="s">
+        <v>32</v>
       </c>
       <c r="F22">
+        <v>120</v>
+      </c>
+      <c r="G22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -997,19 +1098,22 @@
         <v>52</v>
       </c>
       <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
         <v>53</v>
       </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23">
-        <v>120</v>
+      <c r="E23" t="s">
+        <v>32</v>
       </c>
       <c r="F23">
+        <v>120</v>
+      </c>
+      <c r="G23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1017,19 +1121,22 @@
         <v>58</v>
       </c>
       <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
         <v>59</v>
       </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24">
-        <v>120</v>
+      <c r="E24" t="s">
+        <v>32</v>
       </c>
       <c r="F24">
+        <v>120</v>
+      </c>
+      <c r="G24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1037,19 +1144,22 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
         <v>47</v>
       </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25">
-        <v>120</v>
+      <c r="E25" t="s">
+        <v>32</v>
       </c>
       <c r="F25">
+        <v>120</v>
+      </c>
+      <c r="G25">
         <v>0.67</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1057,19 +1167,22 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26">
-        <v>120</v>
+      <c r="E26" t="s">
+        <v>32</v>
       </c>
       <c r="F26">
+        <v>120</v>
+      </c>
+      <c r="G26">
         <v>0.67</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1077,19 +1190,22 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
         <v>55</v>
       </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27">
-        <v>120</v>
+      <c r="E27" t="s">
+        <v>32</v>
       </c>
       <c r="F27">
+        <v>120</v>
+      </c>
+      <c r="G27">
         <v>0.67</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1097,23 +1213,29 @@
         <v>56</v>
       </c>
       <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
         <v>57</v>
       </c>
-      <c r="D28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28">
-        <v>120</v>
+      <c r="E28" t="s">
+        <v>32</v>
       </c>
       <c r="F28">
+        <v>120</v>
+      </c>
+      <c r="G28">
         <v>0.67</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B22:F28">
-    <sortCondition descending="1" ref="F21:F28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B22:G28">
+    <sortCondition descending="1" ref="G21:G28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Småfiksar, funksjon for DBH-uttrekk og endring i malfiler/variabelfiler
</commit_message>
<xml_diff>
--- a/base/OsloMet_paraplyprogram.xlsx
+++ b/base/OsloMet_paraplyprogram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B791EC-F160-4A32-94A9-C93887858CF3}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7A2661F-3F4B-45EE-8EE3-A92DFF34E3C6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
   <si>
     <t>Studieprogramkode</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Paraplyvennleg_kode</t>
   </si>
   <si>
-    <t>MAVIT</t>
-  </si>
-  <si>
     <t>Nivåkode</t>
   </si>
   <si>
@@ -225,16 +222,25 @@
     <t>Paraplynamn</t>
   </si>
   <si>
-    <t>MAVIT Helsevitenskap</t>
-  </si>
-  <si>
-    <t>MASY Spesialsykepleie</t>
-  </si>
-  <si>
     <t>MSFH Sosialfag (H)</t>
   </si>
   <si>
     <t>MSFD Sosialfag (D)</t>
+  </si>
+  <si>
+    <t>SHA Spesialsykepleie</t>
+  </si>
+  <si>
+    <t>MAVIT-RHT</t>
+  </si>
+  <si>
+    <t>MAVIT-SHA</t>
+  </si>
+  <si>
+    <t>RHT Helsevitenskap</t>
+  </si>
+  <si>
+    <t>SHA Helsevitenskap</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,36 +598,36 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>120</v>
@@ -632,19 +638,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>120</v>
@@ -655,65 +661,65 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>120</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <v>120</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>120</v>
@@ -724,65 +730,65 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>120</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8">
         <v>120</v>
       </c>
       <c r="G8">
-        <v>0.67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9">
         <v>120</v>
@@ -793,42 +799,42 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10">
         <v>120</v>
       </c>
       <c r="G10">
-        <v>0.67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11">
         <v>120</v>
@@ -839,19 +845,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12">
         <v>120</v>
@@ -862,65 +868,65 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13">
         <v>120</v>
       </c>
       <c r="G13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14">
         <v>120</v>
       </c>
       <c r="G14">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15">
         <v>120</v>
@@ -931,19 +937,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16">
         <v>120</v>
@@ -954,19 +960,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17">
         <v>120</v>
@@ -977,19 +983,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18">
         <v>120</v>
@@ -1000,19 +1006,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19">
         <v>120</v>
@@ -1023,19 +1029,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
         <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20">
         <v>120</v>
@@ -1046,19 +1052,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21">
         <v>120</v>
@@ -1069,19 +1075,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22">
         <v>120</v>
@@ -1092,19 +1098,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
         <v>52</v>
       </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23">
         <v>120</v>
@@ -1115,19 +1121,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
         <v>58</v>
       </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
-      </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24">
         <v>120</v>
@@ -1138,19 +1144,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
-      </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25">
         <v>120</v>
@@ -1161,19 +1167,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
-      </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26">
         <v>120</v>
@@ -1184,19 +1190,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
         <v>54</v>
       </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>55</v>
-      </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27">
         <v>120</v>
@@ -1207,19 +1213,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" t="s">
-        <v>57</v>
-      </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28">
         <v>120</v>

</xml_diff>

<commit_message>
Oppdatert fil med studieprograminformasjon
</commit_message>
<xml_diff>
--- a/base/OsloMet_paraplyprogram.xlsx
+++ b/base/OsloMet_paraplyprogram.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7A2661F-3F4B-45EE-8EE3-A92DFF34E3C6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,20 +577,20 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" customWidth="1"/>
     <col min="4" max="4" width="104" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -613,7 +613,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -636,7 +636,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -659,7 +659,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -705,7 +705,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -751,7 +751,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -820,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -843,7 +843,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -912,7 +912,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -981,7 +981,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Endringar frå arbeid med studiestartundersøkinga
</commit_message>
<xml_diff>
--- a/base/OsloMet_paraplyprogram.xlsx
+++ b/base/OsloMet_paraplyprogram.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7A2661F-3F4B-45EE-8EE3-A92DFF34E3C6}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC10487E699A650C5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CEE126C-4A72-42E2-9557-9D3EFFC2C8C3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -222,12 +222,6 @@
     <t>Paraplynamn</t>
   </si>
   <si>
-    <t>MSFH Sosialfag (H)</t>
-  </si>
-  <si>
-    <t>MSFD Sosialfag (D)</t>
-  </si>
-  <si>
     <t>SHA Spesialsykepleie</t>
   </si>
   <si>
@@ -241,6 +235,12 @@
   </si>
   <si>
     <t>SHA Helsevitenskap</t>
+  </si>
+  <si>
+    <t>SOS Sosialfag (H)</t>
+  </si>
+  <si>
+    <t>SOS Sosialfag (D)</t>
   </si>
 </sst>
 </file>
@@ -576,21 +576,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
     <col min="4" max="4" width="104" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -613,15 +611,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -636,15 +634,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -659,15 +657,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -682,15 +680,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -705,15 +703,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -728,15 +726,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -751,15 +749,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -774,15 +772,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -797,15 +795,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -820,15 +818,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -843,15 +841,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -866,15 +864,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -889,15 +887,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -912,7 +910,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -920,7 +918,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -935,7 +933,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -943,7 +941,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -958,7 +956,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -966,7 +964,7 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
@@ -981,7 +979,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -989,7 +987,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
@@ -1004,7 +1002,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1012,7 +1010,7 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -1027,7 +1025,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1035,7 +1033,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -1050,7 +1048,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1058,7 +1056,7 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
         <v>44</v>
@@ -1073,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1081,7 +1079,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>48</v>
@@ -1096,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1104,7 +1102,7 @@
         <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>52</v>
@@ -1119,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1127,7 +1125,7 @@
         <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
         <v>58</v>
@@ -1142,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -1150,7 +1148,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
@@ -1165,7 +1163,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1173,7 +1171,7 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>50</v>
@@ -1188,7 +1186,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1196,7 +1194,7 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -1211,7 +1209,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1219,7 +1217,7 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
         <v>56</v>

</xml_diff>